<commit_message>
Modified Baukau Example: One sheet for more detailed specification of catchment types added (surface_rough)
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20383"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E476B2-2083-4373-B113-2169FB4124A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62D09F3-04CE-4104-8BBE-BC7D20AE2BE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="4" r:id="rId2"/>
-    <sheet name="surface_data" sheetId="2" r:id="rId3"/>
+    <sheet name="surface_rough" sheetId="4" r:id="rId2"/>
+    <sheet name="surface_detail" sheetId="2" r:id="rId3"/>
     <sheet name="pollution_data" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="132">
   <si>
     <t>Parameter</t>
   </si>
@@ -397,88 +397,31 @@
     <t>Versiegelte Ableitung</t>
   </si>
   <si>
-    <t>Ebene 1</t>
-  </si>
-  <si>
-    <t>Ebene 2</t>
-  </si>
-  <si>
-    <t>Ebene 3</t>
-  </si>
-  <si>
-    <t>Angeschlossene Fläche</t>
-  </si>
-  <si>
-    <t>Gewerbe und Industrie</t>
-  </si>
-  <si>
-    <t>Fläche abz- Metalldächer</t>
-  </si>
-  <si>
-    <t>Straßen</t>
-  </si>
-  <si>
-    <t>Wenig befahren</t>
-  </si>
-  <si>
-    <t>Einfamilienhäuser</t>
-  </si>
-  <si>
-    <t>Innenstadt Altbau</t>
-  </si>
-  <si>
-    <t>Innenstadt Neubau</t>
-  </si>
-  <si>
-    <t>Fläche</t>
-  </si>
-  <si>
-    <t>Davon behandelt</t>
-  </si>
-  <si>
     <t>Nur an Trennsystem, nicht Mischsystem</t>
   </si>
   <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Hier eine Mischung aus allen Ogre-Kategoriene ("typische" Mischung)</t>
-  </si>
-  <si>
-    <t>kann weg</t>
-  </si>
-  <si>
-    <t>cavon Metalldächer</t>
-  </si>
-  <si>
-    <t>davon Viel befahren</t>
-  </si>
-  <si>
-    <t>Alle angaben in ha</t>
-  </si>
-  <si>
-    <t>Falls eine Unterkategorie nicht angegeben wird, wird ein OgRe- Standardwert angenommen</t>
-  </si>
-  <si>
-    <t>&gt; Standard Gewerbe</t>
-  </si>
-  <si>
-    <t>&gt; Standard Gesamt</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>&gt; Standard EFH</t>
-  </si>
-  <si>
-    <t>&gt; Standard ALT</t>
-  </si>
-  <si>
-    <t>&gt; Standard NEU</t>
-  </si>
-  <si>
-    <t>Ich würde die Konzentrationsmittelwerte gerne über die Fracht berechnen und nicht über die Konzentrationen</t>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>share_percent</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>traffic</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>connected_percent</t>
+  </si>
+  <si>
+    <t>residential_city</t>
+  </si>
+  <si>
+    <t>residential_suburban</t>
   </si>
 </sst>
 </file>
@@ -779,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -905,6 +848,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1213,7 +1160,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1616,7 +1563,7 @@
         <v>35</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1649,127 +1596,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="62">
+        <f>(0.91+0.86)/2</f>
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="C2" s="63">
+        <v>40</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="63">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="62">
+        <v>0.86</v>
+      </c>
+      <c r="C3" s="63">
+        <v>40</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="63">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
+      <c r="B4" s="62">
+        <v>0.91</v>
+      </c>
+      <c r="C4" s="63">
+        <v>20</v>
+      </c>
+      <c r="D4" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>150</v>
+      <c r="E4" s="63">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1689,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1987,7 +1894,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modify loading area types is now based on the excel sheet "surface_areaType"
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62D09F3-04CE-4104-8BBE-BC7D20AE2BE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9360D0-3190-4B4E-AA23-C8C99C68F852}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
-    <sheet name="surface_rough" sheetId="4" r:id="rId2"/>
+    <sheet name="surface_areaType" sheetId="4" r:id="rId2"/>
     <sheet name="surface_detail" sheetId="2" r:id="rId3"/>
     <sheet name="pollution_data" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -812,46 +812,46 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1192,12 +1192,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="64"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
@@ -1248,12 +1248,12 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1386,12 +1386,12 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1517,12 +1517,12 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
@@ -1611,71 +1611,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="52" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="50">
         <f>(0.91+0.86)/2</f>
         <v>0.88500000000000001</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="51">
         <v>40</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="63">
+      <c r="E2" s="51">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="50">
         <v>0.86</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="51">
         <v>40</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="51">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="50">
         <v>0.91</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="51">
         <v>20</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="51">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify manual data input script and all functions related to manual data input
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3532F79-443A-49AC-B714-FDCCCCFF5226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F041E0E-42FE-4812-A108-1307EA081F1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
-    <sheet name="connected_areaType" sheetId="4" r:id="rId2"/>
+    <sheet name="Catchment_LanduseMix" sheetId="4" r:id="rId2"/>
     <sheet name="pollution_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -303,9 +303,6 @@
     <t>connected area in river catchment</t>
   </si>
   <si>
-    <t>seperate_sewer_percent</t>
-  </si>
-  <si>
     <t>Catchment Data</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>landuse</t>
+  </si>
+  <si>
+    <t>separate_sewer_percent</t>
   </si>
 </sst>
 </file>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="7">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>13</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
@@ -1182,7 +1182,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="8">
-        <v>100</v>
+        <v>5.2619999999999996</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>22</v>
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1342,7 +1342,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>46</v>
@@ -1351,7 +1351,7 @@
         <v>88</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1384,7 +1384,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="26">
         <v>0.73</v>

</xml_diff>

<commit_message>
Add "main_road" as additional landuse type. Also modifiy fD value to area-proportional instead of flow proportional.
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20385"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F041E0E-42FE-4812-A108-1307EA081F1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B30FD82-F21C-4CB6-8827-73C3AE096DD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
   <si>
     <t>Parameter</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>separate_sewer_percent</t>
+  </si>
+  <si>
+    <t>main_road</t>
   </si>
 </sst>
 </file>
@@ -1326,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,10 +1365,10 @@
         <v>0.75</v>
       </c>
       <c r="C2" s="27">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D2" s="27">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1379,7 +1382,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="27">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1393,7 +1396,21 @@
         <v>20</v>
       </c>
       <c r="D4" s="27">
-        <v>25</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="27">
+        <v>10</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify variable names and functions
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B30FD82-F21C-4CB6-8827-73C3AE096DD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5011E6F9-AEBE-4EE0-8B00-2D856624FBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
-    <sheet name="Catchment_LanduseMix" sheetId="4" r:id="rId2"/>
-    <sheet name="pollution_data" sheetId="3" r:id="rId3"/>
+    <sheet name="urban_catchment_landuse" sheetId="4" r:id="rId2"/>
+    <sheet name="planning_area_details" sheetId="5" r:id="rId3"/>
+    <sheet name="pollution_data" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="area_plan">site_data!$C$20</definedName>
+    <definedName name="area_plan">site_data!$C$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
   <si>
     <t>Parameter</t>
   </si>
@@ -45,21 +46,9 @@
     <t>Name of surface water body</t>
   </si>
   <si>
-    <t>SUW_type</t>
-  </si>
-  <si>
-    <t>river</t>
-  </si>
-  <si>
-    <t>river or lake?</t>
-  </si>
-  <si>
     <t>LAWA_type</t>
   </si>
   <si>
-    <t>LAWA type of surface water body</t>
-  </si>
-  <si>
     <t>Q_mean</t>
   </si>
   <si>
@@ -93,9 +82,6 @@
     <t>km2</t>
   </si>
   <si>
-    <t>river catchment area</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -117,205 +103,199 @@
     <t>area_plan</t>
   </si>
   <si>
+    <t>Obligatory</t>
+  </si>
+  <si>
+    <t>Natural run-off of urban area ("area_catch") for a yearly rain event</t>
+  </si>
+  <si>
+    <t>Natural run-off of urban area ("area_catch") for a  biennial rain event</t>
+  </si>
+  <si>
+    <t>Average slope of the catchment area</t>
+  </si>
+  <si>
+    <t>River and Rain Data</t>
+  </si>
+  <si>
+    <t>slope_catch</t>
+  </si>
+  <si>
+    <t>Hq1pnat_catch</t>
+  </si>
+  <si>
+    <t>Hq2pnat_catch</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>fD</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Anthracen</t>
+  </si>
+  <si>
+    <t>ug/L</t>
+  </si>
+  <si>
+    <t>measured at 2 points, always below dl</t>
+  </si>
+  <si>
+    <t>Cadmium gelöst</t>
+  </si>
+  <si>
+    <t>measured at 3 points</t>
+  </si>
+  <si>
+    <t>Carbendazim</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>not measured</t>
+  </si>
+  <si>
+    <t>Diethylhexylphthalat (DEHP)</t>
+  </si>
+  <si>
+    <t>Mecoprop</t>
+  </si>
+  <si>
+    <t>Phenanthren</t>
+  </si>
+  <si>
+    <t>measured at 2 points</t>
+  </si>
+  <si>
+    <t>Diuron</t>
+  </si>
+  <si>
+    <t>Fluoranthen</t>
+  </si>
+  <si>
+    <t>Blei gelöst</t>
+  </si>
+  <si>
+    <t>Naphthalin</t>
+  </si>
+  <si>
+    <t>Nickel gelöst</t>
+  </si>
+  <si>
+    <t>Benzo[a]pyren</t>
+  </si>
+  <si>
+    <t>Benzo[b]fluoranthen</t>
+  </si>
+  <si>
+    <t>Benzo[k]fluoranthen</t>
+  </si>
+  <si>
+    <t>Benzo[g,h,i]perylen</t>
+  </si>
+  <si>
+    <t>Terbutryn</t>
+  </si>
+  <si>
+    <t>Zink gelöst</t>
+  </si>
+  <si>
+    <t>Kupfer gelöst</t>
+  </si>
+  <si>
+    <t>AFS fein (&lt;63µm)</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>Orthophosphat</t>
+  </si>
+  <si>
+    <t>measured at 1 point</t>
+  </si>
+  <si>
+    <t>Gesamt-Phosphor</t>
+  </si>
+  <si>
+    <t>Background Concentration</t>
+  </si>
+  <si>
+    <t>Name of the location</t>
+  </si>
+  <si>
+    <t>x_coordinate</t>
+  </si>
+  <si>
+    <t>y_coordinate</t>
+  </si>
+  <si>
+    <t>x value in ETRS 89 - Coordinate System</t>
+  </si>
+  <si>
+    <t>y value in ETRS 89 - Coordinate System</t>
+  </si>
+  <si>
+    <t>City_name</t>
+  </si>
+  <si>
+    <t>Substance</t>
+  </si>
+  <si>
+    <t>residential_city</t>
+  </si>
+  <si>
+    <t>residential_suburban</t>
+  </si>
+  <si>
+    <t>Catchment Data</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>landuse</t>
+  </si>
+  <si>
+    <t>main_road</t>
+  </si>
+  <si>
+    <t>Complete river catchment area upstream of planning area</t>
+  </si>
+  <si>
+    <t>Herne Baukau</t>
+  </si>
+  <si>
+    <t>area_urban</t>
+  </si>
+  <si>
+    <t>urbanised area around planning area</t>
+  </si>
+  <si>
+    <t>no_runoff</t>
+  </si>
+  <si>
+    <t>separate_sewer</t>
+  </si>
+  <si>
+    <t>proportion</t>
+  </si>
+  <si>
+    <t>LAWA type of surface water body (if unkown enter "default")</t>
+  </si>
+  <si>
     <t>planing area</t>
   </si>
   <si>
-    <t>connected impervious area in planing area</t>
-  </si>
-  <si>
-    <t>Obligatory</t>
-  </si>
-  <si>
-    <t>Wie wird das berechnet?</t>
-  </si>
-  <si>
-    <t>Natural run-off of urban area ("area_catch") for a yearly rain event</t>
-  </si>
-  <si>
-    <t>Natural run-off of urban area ("area_catch") for a  biennial rain event</t>
-  </si>
-  <si>
-    <t>Average slope of the catchment area</t>
-  </si>
-  <si>
-    <t>River and Rain Data</t>
-  </si>
-  <si>
-    <t>Vielleicht aus Kostra Daten? Vielleicht müssen eher long und lat angegeben werden</t>
-  </si>
-  <si>
-    <t>Planing Area Data</t>
-  </si>
-  <si>
-    <t>slope_catch</t>
-  </si>
-  <si>
-    <t>Hq1pnat_catch</t>
-  </si>
-  <si>
-    <t>Hq2pnat_catch</t>
-  </si>
-  <si>
-    <t>area_con_catch</t>
-  </si>
-  <si>
-    <t>area_con_plan</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>fD</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Anthracen</t>
-  </si>
-  <si>
-    <t>ug/L</t>
-  </si>
-  <si>
-    <t>measured at 2 points, always below dl</t>
-  </si>
-  <si>
-    <t>Cadmium gelöst</t>
-  </si>
-  <si>
-    <t>measured at 3 points</t>
-  </si>
-  <si>
-    <t>Carbendazim</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>not measured</t>
-  </si>
-  <si>
-    <t>Diethylhexylphthalat (DEHP)</t>
-  </si>
-  <si>
-    <t>Mecoprop</t>
-  </si>
-  <si>
-    <t>Phenanthren</t>
-  </si>
-  <si>
-    <t>measured at 2 points</t>
-  </si>
-  <si>
-    <t>Diuron</t>
-  </si>
-  <si>
-    <t>Fluoranthen</t>
-  </si>
-  <si>
-    <t>Blei gelöst</t>
-  </si>
-  <si>
-    <t>Naphthalin</t>
-  </si>
-  <si>
-    <t>Nickel gelöst</t>
-  </si>
-  <si>
-    <t>Benzo[a]pyren</t>
-  </si>
-  <si>
-    <t>Benzo[b]fluoranthen</t>
-  </si>
-  <si>
-    <t>Benzo[k]fluoranthen</t>
-  </si>
-  <si>
-    <t>Benzo[g,h,i]perylen</t>
-  </si>
-  <si>
-    <t>Terbutryn</t>
-  </si>
-  <si>
-    <t>Zink gelöst</t>
-  </si>
-  <si>
-    <t>Kupfer gelöst</t>
-  </si>
-  <si>
-    <t>AFS fein (&lt;63µm)</t>
-  </si>
-  <si>
-    <t>mg/L</t>
-  </si>
-  <si>
-    <t>Orthophosphat</t>
-  </si>
-  <si>
-    <t>measured at 1 point</t>
-  </si>
-  <si>
-    <t>Gesamt-Phosphor</t>
-  </si>
-  <si>
-    <t>Background Concentration</t>
-  </si>
-  <si>
-    <t>Name of the location</t>
-  </si>
-  <si>
-    <t>x_coordinate</t>
-  </si>
-  <si>
-    <t>y_coordinate</t>
-  </si>
-  <si>
-    <t>x value in ETRS 89 - Coordinate System</t>
-  </si>
-  <si>
-    <t>y value in ETRS 89 - Coordinate System</t>
-  </si>
-  <si>
-    <t>Herne</t>
-  </si>
-  <si>
-    <t>City_name</t>
-  </si>
-  <si>
-    <t>Dev</t>
-  </si>
-  <si>
-    <t>Substance</t>
-  </si>
-  <si>
-    <t>Nur an Trennsystem, nicht Mischsystem</t>
-  </si>
-  <si>
-    <t>share_percent</t>
-  </si>
-  <si>
-    <t>residential_city</t>
-  </si>
-  <si>
-    <t>residential_suburban</t>
-  </si>
-  <si>
-    <t>connected area in river catchment</t>
-  </si>
-  <si>
-    <t>Catchment Data</t>
-  </si>
-  <si>
-    <t>commercial</t>
-  </si>
-  <si>
-    <t>landuse</t>
-  </si>
-  <si>
-    <t>separate_sewer_percent</t>
-  </si>
-  <si>
-    <t>main_road</t>
+    <t>area_urban_upstream</t>
+  </si>
+  <si>
+    <t>urbanised area further upstream that is not considered in "area_urban"</t>
   </si>
 </sst>
 </file>
@@ -360,7 +340,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,18 +385,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -558,12 +532,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -611,7 +620,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -619,20 +627,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -651,15 +662,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -969,16 +971,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.26953125" customWidth="1"/>
     <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="62" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -986,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -995,19 +997,17 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>85</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="A2" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1024,303 +1024,277 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="7">
+        <v>19</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="C5" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7">
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1400</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.04</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>822</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30">
+        <v>3813634.44</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30">
+        <v>2753912.5</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="7">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="C13" s="8">
+        <v>12.4</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="30">
+        <v>1.26</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="7">
-        <v>822</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31">
-        <v>3813634.44</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31">
-        <v>2753912.5</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5.2619999999999996</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="B15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="30">
+        <v>0.107</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="30">
+        <v>4</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="31">
-        <v>1.651</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="8">
-        <v>130</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="15" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="8">
+        <v>22</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="41">
         <v>0.1</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="D19" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="35">
-        <f>1556295/1000/1000</f>
-        <v>1.556295</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="D20"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="39">
-        <f>548919/1000/1000</f>
-        <v>0.54891899999999993</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D22"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1329,9 +1303,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1340,78 +1314,90 @@
     <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B2" s="26">
         <v>0.75</v>
       </c>
       <c r="C2" s="27">
-        <v>30</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B3" s="26">
         <v>0.71</v>
       </c>
       <c r="C3" s="27">
-        <v>40</v>
+        <v>0.36</v>
       </c>
       <c r="D3" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B4" s="26">
         <v>0.73</v>
       </c>
       <c r="C4" s="27">
-        <v>20</v>
+        <v>0.21</v>
       </c>
       <c r="D4" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B5" s="26">
-        <v>0.6</v>
+        <v>0.94</v>
       </c>
       <c r="C5" s="27">
-        <v>10</v>
+        <v>0.05</v>
       </c>
       <c r="D5" s="27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="34">
         <v>0</v>
       </c>
+      <c r="C6" s="27">
+        <v>0.33</v>
+      </c>
+      <c r="D6" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1419,6 +1405,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -1436,310 +1436,310 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C2" s="22">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C3" s="22">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C7" s="22">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C9" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C10" s="22">
         <v>0.186</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C11" s="22">
         <v>1.6E-2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C12" s="22">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C13" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C14" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" s="22">
         <v>2E-3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C18" s="22">
         <v>4.742</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C19" s="22">
         <v>2.1920000000000002</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C21" s="22">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C22" s="23">
         <v>0.108</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify plot script to new data structure.
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5011E6F9-AEBE-4EE0-8B00-2D856624FBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D4AEFE-D35C-4F01-B9BE-25D230B8730C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>Parameter</t>
   </si>
@@ -296,6 +296,72 @@
   </si>
   <si>
     <t>urbanised area further upstream that is not considered in "area_urban"</t>
+  </si>
+  <si>
+    <t>Funktion</t>
+  </si>
+  <si>
+    <t>Eigenschaften</t>
+  </si>
+  <si>
+    <t>Wohngebäude</t>
+  </si>
+  <si>
+    <t>In Verkehrsreichem Gebiet</t>
+  </si>
+  <si>
+    <t>Mit Zinkdach</t>
+  </si>
+  <si>
+    <t>Mit Gründach</t>
+  </si>
+  <si>
+    <t>Mit Biozidverwendung / unbekannt</t>
+  </si>
+  <si>
+    <t>Ohne Biozidverwendung</t>
+  </si>
+  <si>
+    <t>Mit Bitumendach</t>
+  </si>
+  <si>
+    <t>Mit Ziegel-, Glas-, sonstiges Metalldach, etc.</t>
+  </si>
+  <si>
+    <t>In Verkehrsarmen Gebiet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gewerbe/Industriegebäude </t>
+  </si>
+  <si>
+    <t>Mit Biozidverwendung</t>
+  </si>
+  <si>
+    <t>Hoffläche</t>
+  </si>
+  <si>
+    <t>Fugenlos</t>
+  </si>
+  <si>
+    <t>offene Fugen</t>
+  </si>
+  <si>
+    <t>Straße</t>
+  </si>
+  <si>
+    <t>Viel befahren</t>
+  </si>
+  <si>
+    <t>Mittel befahren</t>
+  </si>
+  <si>
+    <t>gering befahren</t>
+  </si>
+  <si>
+    <t>kaum befahren</t>
+  </si>
+  <si>
+    <t>area_m2</t>
   </si>
 </sst>
 </file>
@@ -572,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -646,6 +712,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,6 +732,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -972,7 +1048,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,12 +1078,12 @@
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1112,12 +1188,12 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1227,7 +1303,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>89</v>
@@ -1306,7 +1382,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,14 +1482,444 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="43"/>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="43"/>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="51"/>
+      <c r="B25" s="51"/>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="43"/>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="43"/>
+      <c r="E26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="43"/>
+      <c r="E27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="51"/>
+      <c r="B28" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="43"/>
+      <c r="E28">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="C29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="43"/>
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="51"/>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="51"/>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="51"/>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ADD Beispiele und Plots Abschlussveranstaltung
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau.xlsx
+++ b/inst/extdata/Data_entry/Baukau.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amatzi\Documents\github-repos\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5011E6F9-AEBE-4EE0-8B00-2D856624FBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6ECE47-C808-4998-BB95-8CBE2E7A0450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="28524" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
@@ -972,18 +972,18 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="62" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>29</v>
       </c>
@@ -1010,7 +1010,7 @@
       <c r="D2" s="45"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>13</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>1400</v>
+        <v>5000</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>15</v>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>19</v>
       </c>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>75</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="D9" s="48"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>71</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>67</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>68</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>16</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="8">
-        <v>12.4</v>
+        <v>5.2</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>79</v>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>81</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>24</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="30">
-        <v>0.107</v>
+        <v>1.26</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>87</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>88</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>89</v>
@@ -1235,7 +1235,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>31</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>32</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
@@ -1279,16 +1279,16 @@
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22"/>
     </row>
   </sheetData>
@@ -1309,15 +1309,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>77</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>73</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>74</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>76</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>78</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>83</v>
       </c>
@@ -1412,7 +1412,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1426,15 +1426,15 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>72</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>45</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>48</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>50</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>57</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>58</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>59</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>60</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>62</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>64</v>
       </c>

</xml_diff>